<commit_message>
created Service, ServiceImpl, DAO and DAOImpl. Cleaned IT Tests. Closes #14.
</commit_message>
<xml_diff>
--- a/src/main/resources/WriteSheet.xlsx
+++ b/src/main/resources/WriteSheet.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="11">
   <si>
     <t>Sort Algorithm</t>
   </si>
@@ -26,7 +26,7 @@
     <t>BubbleSort</t>
   </si>
   <si>
-    <t>3</t>
+    <t>5</t>
   </si>
   <si>
     <t>0</t>
@@ -119,18 +119,18 @@
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="B3" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C3" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B4" t="s">
         <v>4</v>
@@ -141,18 +141,18 @@
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="B5" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C5" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B6" t="s">
         <v>4</v>
@@ -163,67 +163,12 @@
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="B7" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C7" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="s">
-        <v>8</v>
-      </c>
-      <c r="B8" t="s">
-        <v>4</v>
-      </c>
-      <c r="C8" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="s">
-        <v>0</v>
-      </c>
-      <c r="B9" t="s">
-        <v>1</v>
-      </c>
-      <c r="C9" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="s">
-        <v>9</v>
-      </c>
-      <c r="B10" t="s">
-        <v>4</v>
-      </c>
-      <c r="C10" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="s">
-        <v>0</v>
-      </c>
-      <c r="B11" t="s">
-        <v>1</v>
-      </c>
-      <c r="C11" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="s">
-        <v>10</v>
-      </c>
-      <c r="B12" t="s">
-        <v>4</v>
-      </c>
-      <c r="C12" t="s">
         <v>5</v>
       </c>
     </row>

</xml_diff>

<commit_message>
integrated Spring AOP for sort(), service layer and dao layer. Closes #2.
</commit_message>
<xml_diff>
--- a/src/main/resources/WriteSheet.xlsx
+++ b/src/main/resources/WriteSheet.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="9">
   <si>
     <t>Sort Algorithm</t>
   </si>
@@ -23,31 +23,22 @@
     <t>Time Taken</t>
   </si>
   <si>
-    <t>BubbleSort</t>
+    <t>$Proxy21</t>
   </si>
   <si>
     <t>5</t>
   </si>
   <si>
+    <t>7</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
     <t>1</t>
   </si>
   <si>
-    <t>InsertionSort</t>
-  </si>
-  <si>
-    <t>0</t>
-  </si>
-  <si>
-    <t>MergeSort</t>
-  </si>
-  <si>
-    <t>QuickSort</t>
-  </si>
-  <si>
-    <t>SelectionSort</t>
-  </si>
-  <si>
-    <t>ShellSort</t>
+    <t>3</t>
   </si>
 </sst>
 </file>
@@ -122,18 +113,18 @@
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B3" t="s">
         <v>4</v>
       </c>
       <c r="C3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="B4" t="s">
         <v>4</v>
@@ -144,7 +135,7 @@
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="B5" t="s">
         <v>4</v>
@@ -155,18 +146,18 @@
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="B6" t="s">
         <v>4</v>
       </c>
       <c r="C6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>11</v>
+        <v>3</v>
       </c>
       <c r="B7" t="s">
         <v>4</v>

</xml_diff>